<commit_message>
changed most of the cucumber fixtures into rspec test cases. more to go.
</commit_message>
<xml_diff>
--- a/design docs/stuff.xlsx
+++ b/design docs/stuff.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$1</definedName>
+  </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="59">
   <si>
     <t>User</t>
   </si>
@@ -190,6 +193,12 @@
   </si>
   <si>
     <t>change themes</t>
+  </si>
+  <si>
+    <t>add registry items</t>
+  </si>
+  <si>
+    <t>Delete registry items</t>
   </si>
 </sst>
 </file>
@@ -330,8 +339,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B53" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="A1:B53"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B55" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A1:B55"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Functionality" dataDxfId="3"/>
     <tableColumn id="2" name="Level" dataDxfId="2"/>
@@ -662,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -808,7 +817,7 @@
     </row>
     <row r="18" spans="1:2" ht="20">
       <c r="A18" s="2" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>50</v>
@@ -816,7 +825,7 @@
     </row>
     <row r="19" spans="1:2" ht="20">
       <c r="A19" s="2" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>50</v>
@@ -824,7 +833,7 @@
     </row>
     <row r="20" spans="1:2" ht="20">
       <c r="A20" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>50</v>
@@ -832,7 +841,7 @@
     </row>
     <row r="21" spans="1:2" ht="20">
       <c r="A21" s="2" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>50</v>
@@ -840,7 +849,7 @@
     </row>
     <row r="22" spans="1:2" ht="20">
       <c r="A22" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>50</v>
@@ -848,7 +857,7 @@
     </row>
     <row r="23" spans="1:2" ht="20">
       <c r="A23" s="2" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>50</v>
@@ -856,7 +865,7 @@
     </row>
     <row r="24" spans="1:2" ht="20">
       <c r="A24" s="2" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>50</v>
@@ -864,23 +873,23 @@
     </row>
     <row r="25" spans="1:2" ht="20">
       <c r="A25" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="20">
       <c r="A26" s="2" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="20">
       <c r="A27" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>53</v>
@@ -888,15 +897,15 @@
     </row>
     <row r="28" spans="1:2" ht="20">
       <c r="A28" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="20">
       <c r="A29" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>53</v>
@@ -904,37 +913,37 @@
     </row>
     <row r="30" spans="1:2" ht="20">
       <c r="A30" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="20">
+      <c r="A31" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" ht="20">
-      <c r="A31" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" s="2"/>
     </row>
     <row r="32" spans="1:2" ht="20">
       <c r="A32" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="20">
-      <c r="A33" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="A33" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="2"/>
     </row>
     <row r="34" spans="1:2" ht="20">
       <c r="A34" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>50</v>
@@ -942,7 +951,7 @@
     </row>
     <row r="35" spans="1:2" ht="20">
       <c r="A35" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>50</v>
@@ -950,143 +959,160 @@
     </row>
     <row r="36" spans="1:2" ht="20">
       <c r="A36" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="20">
-      <c r="A37" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B37" s="2"/>
+      <c r="A37" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="38" spans="1:2" ht="20">
       <c r="A38" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="20">
       <c r="A39" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B39" s="2"/>
     </row>
     <row r="40" spans="1:2" ht="20">
       <c r="A40" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="20">
-      <c r="A41" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="A41" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" s="2"/>
     </row>
     <row r="42" spans="1:2" ht="20">
       <c r="A42" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B42" s="2">
-        <v>2</v>
+        <v>35</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="20">
       <c r="A43" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="20">
-      <c r="A44" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B44" s="2"/>
+      <c r="A44" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B44" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="45" spans="1:2" ht="20">
       <c r="A45" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="20">
-      <c r="A46" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B46" s="2">
-        <v>2</v>
-      </c>
+      <c r="A46" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B46" s="2"/>
     </row>
     <row r="47" spans="1:2" ht="20">
       <c r="A47" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B47" s="2">
-        <v>2</v>
+        <v>40</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="20">
       <c r="A48" s="2" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="B48" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="20">
-      <c r="A49" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B49" s="2"/>
+      <c r="A49" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B49" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="50" spans="1:2" ht="20">
       <c r="A50" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B50" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="20">
-      <c r="A51" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B51" s="2">
-        <v>2</v>
-      </c>
+      <c r="A51" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B51" s="2"/>
     </row>
     <row r="52" spans="1:2" ht="20">
       <c r="A52" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
+      </c>
+      <c r="B52" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="20">
       <c r="A53" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B53" s="2">
         <v>2</v>
       </c>
     </row>
+    <row r="54" spans="1:2" ht="20">
+      <c r="A54" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="20">
+      <c r="A55" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B55" s="2">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Guard is now running, and most of the work now done around the basic item attributes. next is to do the associations between registry_items and attr_names through an item_attr_value model
</commit_message>
<xml_diff>
--- a/design docs/stuff.xlsx
+++ b/design docs/stuff.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="61">
   <si>
     <t>User</t>
   </si>
@@ -199,6 +199,12 @@
   </si>
   <si>
     <t>Delete registry items</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -276,19 +282,15 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="18"/>
+        <sz val="16"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
@@ -333,17 +335,35 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B55" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="A1:B55"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Functionality" dataDxfId="3"/>
-    <tableColumn id="2" name="Level" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C55" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C55"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Functionality" dataDxfId="2"/>
+    <tableColumn id="2" name="Level" dataDxfId="1"/>
+    <tableColumn id="3" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -671,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B55"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -683,431 +703,500 @@
     <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="4" customFormat="1" ht="23">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="23">
       <c r="A1" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="20">
+      <c r="C1" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="20">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:2" ht="20">
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" ht="20">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="20">
+      <c r="C3" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="20">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="20">
+      <c r="C4" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="20">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="20">
+      <c r="C5" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="20">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="20">
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" ht="20">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="20">
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" ht="20">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="20">
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" ht="20">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="20">
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" ht="20">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="20">
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" ht="20">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:2" ht="20">
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" ht="20">
       <c r="A12" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="20">
+      <c r="C12" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="20">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="20">
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" ht="20">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="20">
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" ht="20">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" ht="20">
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" ht="20">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="20">
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" ht="20">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="20">
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:3" ht="20">
       <c r="A18" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="20">
+      <c r="C18" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="20">
       <c r="A19" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="20">
+      <c r="C19" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="20">
       <c r="A20" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="20">
+      <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="1:3" ht="20">
       <c r="A21" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="20">
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="1:3" ht="20">
       <c r="A22" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="20">
+      <c r="C22" s="2"/>
+    </row>
+    <row r="23" spans="1:3" ht="20">
       <c r="A23" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="20">
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="1:3" ht="20">
       <c r="A24" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="20">
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" spans="1:3" ht="20">
       <c r="A25" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="20">
+      <c r="C25" s="2"/>
+    </row>
+    <row r="26" spans="1:3" ht="20">
       <c r="A26" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="20">
+      <c r="C26" s="2"/>
+    </row>
+    <row r="27" spans="1:3" ht="20">
       <c r="A27" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="20">
+      <c r="C27" s="2"/>
+    </row>
+    <row r="28" spans="1:3" ht="20">
       <c r="A28" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="20">
+      <c r="C28" s="2"/>
+    </row>
+    <row r="29" spans="1:3" ht="20">
       <c r="A29" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="20">
+      <c r="C29" s="2"/>
+    </row>
+    <row r="30" spans="1:3" ht="20">
       <c r="A30" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" ht="20">
+      <c r="C30" s="2"/>
+    </row>
+    <row r="31" spans="1:3" ht="20">
       <c r="A31" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" ht="20">
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" spans="1:3" ht="20">
       <c r="A32" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="20">
+      <c r="C32" s="2"/>
+    </row>
+    <row r="33" spans="1:3" ht="20">
       <c r="A33" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B33" s="2"/>
-    </row>
-    <row r="34" spans="1:2" ht="20">
+      <c r="C33" s="2"/>
+    </row>
+    <row r="34" spans="1:3" ht="20">
       <c r="A34" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" ht="20">
+      <c r="C34" s="2"/>
+    </row>
+    <row r="35" spans="1:3" ht="20">
       <c r="A35" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" ht="20">
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="1:3" ht="20">
       <c r="A36" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" ht="20">
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="1:3" ht="20">
       <c r="A37" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" ht="20">
+      <c r="C37" s="2"/>
+    </row>
+    <row r="38" spans="1:3" ht="20">
       <c r="A38" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" ht="20">
+      <c r="C38" s="2"/>
+    </row>
+    <row r="39" spans="1:3" ht="20">
       <c r="A39" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B39" s="2"/>
-    </row>
-    <row r="40" spans="1:2" ht="20">
+      <c r="C39" s="2"/>
+    </row>
+    <row r="40" spans="1:3" ht="20">
       <c r="A40" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" ht="20">
+      <c r="C40" s="2"/>
+    </row>
+    <row r="41" spans="1:3" ht="20">
       <c r="A41" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B41" s="2"/>
-    </row>
-    <row r="42" spans="1:2" ht="20">
+      <c r="C41" s="2"/>
+    </row>
+    <row r="42" spans="1:3" ht="20">
       <c r="A42" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" ht="20">
+      <c r="C42" s="2"/>
+    </row>
+    <row r="43" spans="1:3" ht="20">
       <c r="A43" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" ht="20">
+      <c r="C43" s="2"/>
+    </row>
+    <row r="44" spans="1:3" ht="20">
       <c r="A44" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B44" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" ht="20">
+      <c r="C44" s="2"/>
+    </row>
+    <row r="45" spans="1:3" ht="20">
       <c r="A45" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" ht="20">
+      <c r="C45" s="2"/>
+    </row>
+    <row r="46" spans="1:3" ht="20">
       <c r="A46" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B46" s="2"/>
-    </row>
-    <row r="47" spans="1:2" ht="20">
+      <c r="C46" s="2"/>
+    </row>
+    <row r="47" spans="1:3" ht="20">
       <c r="A47" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" ht="20">
+      <c r="C47" s="2"/>
+    </row>
+    <row r="48" spans="1:3" ht="20">
       <c r="A48" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B48" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" ht="20">
+      <c r="C48" s="2"/>
+    </row>
+    <row r="49" spans="1:3" ht="20">
       <c r="A49" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B49" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" ht="20">
+      <c r="C49" s="2"/>
+    </row>
+    <row r="50" spans="1:3" ht="20">
       <c r="A50" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B50" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" ht="20">
+      <c r="C50" s="2"/>
+    </row>
+    <row r="51" spans="1:3" ht="20">
       <c r="A51" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B51" s="2"/>
-    </row>
-    <row r="52" spans="1:2" ht="20">
+      <c r="C51" s="2"/>
+    </row>
+    <row r="52" spans="1:3" ht="20">
       <c r="A52" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B52" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" ht="20">
+      <c r="C52" s="2"/>
+    </row>
+    <row r="53" spans="1:3" ht="20">
       <c r="A53" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B53" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" ht="20">
+      <c r="C53" s="2"/>
+    </row>
+    <row r="54" spans="1:3" ht="20">
       <c r="A54" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" ht="20">
+      <c r="C54" s="2"/>
+    </row>
+    <row r="55" spans="1:3" ht="20">
       <c r="A55" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B55" s="2">
         <v>2</v>
       </c>
+      <c r="C55" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
branched for dodgy code - the select value is not kept on edit, and the money-rails gem has not been implemented fully
</commit_message>
<xml_diff>
--- a/design docs/stuff.xlsx
+++ b/design docs/stuff.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="61">
   <si>
     <t>User</t>
   </si>
@@ -693,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -891,7 +891,9 @@
       <c r="B20" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="2"/>
+      <c r="C20" s="2" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="21" spans="1:3" ht="20">
       <c r="A21" s="2" t="s">
@@ -909,7 +911,9 @@
       <c r="B22" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="2"/>
+      <c r="C22" s="2" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="23" spans="1:3" ht="20">
       <c r="A23" s="2" t="s">
@@ -927,7 +931,9 @@
       <c r="B24" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="2"/>
+      <c r="C24" s="2" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="25" spans="1:3" ht="20">
       <c r="A25" s="2" t="s">
@@ -936,7 +942,9 @@
       <c r="B25" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="2"/>
+      <c r="C25" s="2" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="26" spans="1:3" ht="20">
       <c r="A26" s="2" t="s">

</xml_diff>